<commit_message>
update 12 & 13
</commit_message>
<xml_diff>
--- a/demo overzicht.xlsx
+++ b/demo overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpols\Documents\GitHub\Showing-Physics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228D83FD-A490-4053-8D69-47451D33B79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF2EC3C-2FDD-4BA1-AE9F-390CEABB871A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="1590" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1470" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
   <si>
     <t>demo</t>
   </si>
@@ -585,7 +585,7 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,6 +727,9 @@
       <c r="B13" t="s">
         <v>58</v>
       </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -735,6 +738,9 @@
       <c r="B14" t="s">
         <v>59</v>
       </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -742,6 +748,9 @@
       </c>
       <c r="B15" t="s">
         <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update 26 & 27
</commit_message>
<xml_diff>
--- a/demo overzicht.xlsx
+++ b/demo overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpols\Documents\GitHub\Showing-Physics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAF5D32-CFFE-4785-9DD3-AB76C8F61FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DED3359-E58F-42A5-95F6-6476DA30A0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="1356" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,8 +983,8 @@
       <c r="B26" t="s">
         <v>35</v>
       </c>
-      <c r="D26" t="s">
-        <v>111</v>
+      <c r="C26" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1005,7 +1005,7 @@
       <c r="B28" t="s">
         <v>66</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1016,8 +1016,8 @@
       <c r="B29" t="s">
         <v>23</v>
       </c>
-      <c r="C29" t="s">
-        <v>82</v>
+      <c r="C29" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update 36 and PoE
</commit_message>
<xml_diff>
--- a/demo overzicht.xlsx
+++ b/demo overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpols\Documents\GitHub\Showing-Physics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB52965-D60E-4D48-BEA4-9216E8EB4E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAB75EE-FBFA-4B54-B3E6-97E4764AF511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23496" yWindow="2436" windowWidth="21600" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="111">
   <si>
     <t>demo</t>
   </si>
@@ -358,9 +358,6 @@
   </si>
   <si>
     <t>Miscommunicating vessels</t>
-  </si>
-  <si>
-    <t>betere foto</t>
   </si>
 </sst>
 </file>
@@ -408,10 +405,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,15 +693,15 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="93.7109375" customWidth="1"/>
+    <col min="2" max="2" width="93.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -717,7 +715,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -728,7 +726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -739,7 +737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -750,7 +748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -761,7 +759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -772,7 +770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -783,7 +781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -794,7 +792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -805,7 +803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -816,7 +814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -827,7 +825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -838,7 +836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -849,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -860,7 +858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -871,7 +869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -882,7 +880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -893,7 +891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -904,7 +902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -915,7 +913,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -929,7 +927,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -940,7 +938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -951,7 +949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -962,7 +960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -973,7 +971,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -984,7 +982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -995,7 +993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1006,7 +1004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1017,7 +1015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1028,7 +1026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1039,7 +1037,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1050,7 +1048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1061,7 +1059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1072,7 +1070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1083,18 +1081,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>72</v>
       </c>
-      <c r="D36" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1105,15 +1103,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1124,7 +1125,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1143,7 +1144,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1154,7 +1155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1162,7 +1163,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1173,7 +1174,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1181,7 +1182,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1189,7 +1190,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1197,7 +1198,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1208,7 +1209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1219,7 +1220,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1230,7 +1231,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1238,7 +1239,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1246,7 +1247,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1254,7 +1255,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1265,7 +1266,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1273,7 +1274,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1281,7 +1282,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1289,7 +1290,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1300,7 +1301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1308,7 +1309,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1316,7 +1317,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1327,7 +1328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1335,7 +1336,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -1346,7 +1347,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -1357,7 +1358,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -1368,7 +1369,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -1376,7 +1377,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -1384,7 +1385,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -1392,7 +1393,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -1400,7 +1401,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -1408,7 +1409,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -1416,7 +1417,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -1427,7 +1428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -1438,7 +1439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -1446,7 +1447,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -1454,7 +1455,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -1462,7 +1463,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -1470,7 +1471,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -1478,7 +1479,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -1486,7 +1487,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -1497,7 +1498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
@@ -1505,7 +1506,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
@@ -1513,7 +1514,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
@@ -1521,7 +1522,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
@@ -1529,7 +1530,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -1537,7 +1538,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
@@ -1545,7 +1546,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
@@ -1553,7 +1554,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
@@ -1561,7 +1562,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
@@ -1569,7 +1570,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
@@ -1580,7 +1581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
@@ -1591,7 +1592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
@@ -1602,7 +1603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
@@ -1613,7 +1614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
@@ -1624,7 +1625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
@@ -1635,7 +1636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
@@ -1646,7 +1647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
@@ -1657,7 +1658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>96</v>
       </c>
@@ -1668,7 +1669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>97</v>
       </c>
@@ -1679,7 +1680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>98</v>
       </c>
@@ -1693,7 +1694,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
update 32 53 98
</commit_message>
<xml_diff>
--- a/demo overzicht.xlsx
+++ b/demo overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpols\Documents\GitHub\Showing-Physics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C0E068-50AE-4051-AF21-05DCE79235C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A110060E-4F6F-49CD-937F-4F8343898349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="1356" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="124">
   <si>
     <t>demo</t>
   </si>
@@ -749,15 +749,15 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="93.6640625" customWidth="1"/>
+    <col min="2" max="2" width="93.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -774,7 +774,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>3</v>
       </c>
@@ -782,7 +782,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -794,14 +794,14 @@
       </c>
       <c r="F3">
         <f>COUNTIF(C3:C103,"voltooid")</f>
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G3">
         <f>F1-F3</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -812,7 +812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -823,7 +823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -834,7 +834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -845,7 +845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -856,7 +856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -867,7 +867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -878,7 +878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -889,7 +889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -900,7 +900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -911,7 +911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -922,7 +922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -933,7 +933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -944,7 +944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -955,7 +955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -966,7 +966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -977,7 +977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -988,7 +988,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1389,15 +1389,18 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C55" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1405,7 +1408,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1413,7 +1416,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1424,7 +1427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1432,7 +1435,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1440,7 +1443,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1451,7 +1454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1459,7 +1462,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -1470,7 +1473,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -1508,7 +1511,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -1516,7 +1519,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -1524,7 +1527,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -1532,7 +1535,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -1543,7 +1546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -1554,7 +1557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -1573,7 +1576,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -1584,7 +1587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -1592,7 +1595,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -1600,7 +1603,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -1608,7 +1611,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -1630,7 +1633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -1641,7 +1644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -1652,7 +1655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -1663,7 +1666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -1691,7 +1694,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -1705,7 +1708,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -1716,7 +1719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -1727,7 +1730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -1738,7 +1741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -1749,7 +1752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -1760,7 +1763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -1782,7 +1785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -1793,7 +1796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -1804,7 +1807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -1815,7 +1818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -1826,7 +1829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -1837,7 +1840,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -1848,7 +1851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -1862,7 +1865,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
update 18, 29, 43
</commit_message>
<xml_diff>
--- a/demo overzicht.xlsx
+++ b/demo overzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpols\Documents\GitHub\Showing-Physics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D336A0F-94A0-42FB-998C-870C1C57B071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F246658-2CB1-4A6D-B604-DD21E6E4B969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="122">
   <si>
     <t>demo</t>
   </si>
@@ -353,9 +353,6 @@
     <t>On a roll</t>
   </si>
   <si>
-    <t>nieuwe video</t>
-  </si>
-  <si>
     <t>Miscommunicating vessels</t>
   </si>
   <si>
@@ -365,15 +362,9 @@
     <t>te gaan</t>
   </si>
   <si>
-    <t>maken</t>
-  </si>
-  <si>
     <t>Force and motion with a bowling ball</t>
   </si>
   <si>
-    <t>betere foto</t>
-  </si>
-  <si>
     <t>zou fotos kunnen gebruiken</t>
   </si>
   <si>
@@ -405,6 +396,12 @@
   </si>
   <si>
     <t>fotos</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>foto uncommenten</t>
   </si>
 </sst>
 </file>
@@ -745,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -791,11 +788,11 @@
       </c>
       <c r="F3">
         <f>COUNTIF(C3:C103,"voltooid")</f>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G3">
         <f>F1-F3</f>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1105,8 +1102,8 @@
       <c r="B31" t="s">
         <v>87</v>
       </c>
-      <c r="D31" t="s">
-        <v>105</v>
+      <c r="C31" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1186,7 +1183,7 @@
         <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1205,7 +1202,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>3</v>
@@ -1260,13 +1257,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D45" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="E45" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1280,7 +1277,7 @@
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1294,7 +1291,7 @@
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1324,16 +1321,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D50" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G50" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -1358,7 +1355,7 @@
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -1372,7 +1369,7 @@
         <v>3</v>
       </c>
       <c r="D53" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -1383,7 +1380,7 @@
         <v>91</v>
       </c>
       <c r="D54" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -1680,7 +1677,7 @@
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.35">
@@ -1694,7 +1691,7 @@
         <v>3</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -1708,7 +1705,7 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
final edits demos 58-65
</commit_message>
<xml_diff>
--- a/demo overzicht.xlsx
+++ b/demo overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpols\Documents\GitHub\Showing-Physics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1855EF-E48E-4617-B76A-B87C3832AEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0516E6-E932-4B86-B2C5-29C7D448FCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1470" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="121">
   <si>
     <t>demo</t>
   </si>
@@ -275,9 +275,6 @@
     <t>Implosion</t>
   </si>
   <si>
-    <t>filmpje toevoegen</t>
-  </si>
-  <si>
     <t>Radioactive decay - A simulation</t>
   </si>
   <si>
@@ -347,9 +344,6 @@
     <t>Transit of a planet</t>
   </si>
   <si>
-    <t>nv</t>
-  </si>
-  <si>
     <t>On a roll</t>
   </si>
   <si>
@@ -399,6 +393,12 @@
   </si>
   <si>
     <t>foto uncommenten</t>
+  </si>
+  <si>
+    <t>video?</t>
+  </si>
+  <si>
+    <t>video ballon op blazen en releasen</t>
   </si>
 </sst>
 </file>
@@ -739,16 +739,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="93.6640625" customWidth="1"/>
+    <col min="2" max="2" width="93.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -765,15 +765,15 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -785,14 +785,14 @@
       </c>
       <c r="F3">
         <f>COUNTIF(C3:C103,"voltooid")</f>
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G3">
         <f>F1-F3</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -803,7 +803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -814,7 +814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -825,7 +825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -836,7 +836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -847,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -858,7 +858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -869,7 +869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -880,7 +880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -891,7 +891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -902,7 +902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -913,7 +913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -924,7 +924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -935,7 +935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -946,7 +946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -957,7 +957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -968,7 +968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -979,7 +979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -993,7 +993,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1092,29 +1092,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1125,18 +1125,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1158,18 +1158,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1180,10 +1180,10 @@
         <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1194,18 +1194,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1238,49 +1238,49 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D45" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E45" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1291,10 +1291,10 @@
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1316,24 +1316,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="D50" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G50" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1355,10 +1355,10 @@
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1369,21 +1369,21 @@
         <v>3</v>
       </c>
       <c r="D53" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1394,56 +1394,68 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1454,64 +1466,79 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C62" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="B63" t="s">
         <v>16</v>
       </c>
-      <c r="D63" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C63" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="B64" t="s">
         <v>26</v>
       </c>
-      <c r="D64" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C64" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>98</v>
-      </c>
-      <c r="D65" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="B66" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C66" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
       <c r="B67" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -1519,15 +1546,15 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -1535,7 +1562,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -1546,7 +1573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -1557,7 +1584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -1568,7 +1595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -1576,7 +1603,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -1587,7 +1614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -1595,23 +1622,23 @@
         <v>35</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -1622,7 +1649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -1633,7 +1660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -1644,7 +1671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -1655,7 +1682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -1666,21 +1693,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C84" t="s">
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -1691,10 +1718,10 @@
         <v>3</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -1705,10 +1732,10 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -1719,7 +1746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -1730,7 +1757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -1741,40 +1768,40 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -1785,29 +1812,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -1818,40 +1845,40 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -1861,11 +1888,8 @@
       <c r="C100" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D100" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>

</xml_diff>